<commit_message>
Fixed university images not showing.
</commit_message>
<xml_diff>
--- a/database/seeds/csvs/schools-universities.xlsx
+++ b/database/seeds/csvs/schools-universities.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Downloads\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Poom\ICT\Senior\campass\database\seeds\csvs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A760FB62-E944-4ADF-ACD2-21305AFD179D}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C4BC187F-4626-404A-AB20-0574744CD48D}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="1" xr2:uid="{C55A2BD8-7250-4E84-8D4E-BA2B9FD21431}"/>
   </bookViews>
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1499" uniqueCount="1237">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1562" uniqueCount="1255">
   <si>
     <t>โรงเรียนยะหาศิรยานุกูล</t>
   </si>
@@ -3738,6 +3738,60 @@
   </si>
   <si>
     <t>subtype</t>
+  </si>
+  <si>
+    <t>image</t>
+  </si>
+  <si>
+    <t>KMITL</t>
+  </si>
+  <si>
+    <t>NU</t>
+  </si>
+  <si>
+    <t>KU</t>
+  </si>
+  <si>
+    <t>RMU</t>
+  </si>
+  <si>
+    <t>RU</t>
+  </si>
+  <si>
+    <t>MU</t>
+  </si>
+  <si>
+    <t>SU</t>
+  </si>
+  <si>
+    <t>PSU</t>
+  </si>
+  <si>
+    <t>TU</t>
+  </si>
+  <si>
+    <t>KKU</t>
+  </si>
+  <si>
+    <t>CU</t>
+  </si>
+  <si>
+    <t>CMU</t>
+  </si>
+  <si>
+    <t>KMUTT</t>
+  </si>
+  <si>
+    <t>KMUTNB</t>
+  </si>
+  <si>
+    <t>SUT</t>
+  </si>
+  <si>
+    <t>BUU</t>
+  </si>
+  <si>
+    <t>SWU</t>
   </si>
 </sst>
 </file>
@@ -3854,12 +3908,12 @@
 </file>
 
 <file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{EF0CE763-16FE-4896-B69B-A744111DC284}" name="Table1" displayName="Table1" ref="A1:E199" totalsRowShown="0">
-  <autoFilter ref="A1:E199" xr:uid="{0650E731-3BD5-44E3-AD5D-F07E114B7B88}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{EF0CE763-16FE-4896-B69B-A744111DC284}" name="Table1" displayName="Table1" ref="A1:F199" totalsRowShown="0">
+  <autoFilter ref="A1:F199" xr:uid="{0650E731-3BD5-44E3-AD5D-F07E114B7B88}"/>
   <sortState ref="A2:E199">
     <sortCondition ref="C1:C199"/>
   </sortState>
-  <tableColumns count="5">
+  <tableColumns count="6">
     <tableColumn id="1" xr3:uid="{FF5F1F1B-FBE0-4C0E-95D4-10F615B331B5}" name="name_th"/>
     <tableColumn id="2" xr3:uid="{0FA6B461-1C7A-4A89-851C-44BBB9C9A5B9}" name="name_en"/>
     <tableColumn id="4" xr3:uid="{C79F5DA3-4CA0-4D65-86D4-0A2658A53FF3}" name="subtype_text"/>
@@ -3867,6 +3921,7 @@
       <calculatedColumnFormula>VLOOKUP(Table1[[#This Row],[subtype_text]],Table13[#All],2,FALSE)</calculatedColumnFormula>
     </tableColumn>
     <tableColumn id="3" xr3:uid="{D80B5BB9-BA8D-4DD7-B249-5A9FEB0EF062}" name="remark"/>
+    <tableColumn id="6" xr3:uid="{EC19D0F4-5952-4EC1-B74A-D1912951DCFC}" name="image"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -8354,10 +8409,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{54777062-7541-45FA-8504-632238C86CFC}">
-  <dimension ref="A1:E219"/>
+  <dimension ref="A1:F219"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="J8" sqref="J8"/>
+    <sheetView tabSelected="1" topLeftCell="A130" workbookViewId="0">
+      <selection activeCell="F143" sqref="F143"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -8368,7 +8423,7 @@
     <col min="4" max="4" width="19.7109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5">
+    <row r="1" spans="1:6">
       <c r="A1" t="s">
         <v>1232</v>
       </c>
@@ -8384,8 +8439,11 @@
       <c r="E1" t="s">
         <v>1234</v>
       </c>
-    </row>
-    <row r="2" spans="1:5">
+      <c r="F1" t="s">
+        <v>1237</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6">
       <c r="A2" t="s">
         <v>943</v>
       </c>
@@ -8400,7 +8458,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="3" spans="1:5">
+    <row r="3" spans="1:6">
       <c r="A3" t="s">
         <v>987</v>
       </c>
@@ -8415,7 +8473,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="4" spans="1:5">
+    <row r="4" spans="1:6">
       <c r="A4" t="s">
         <v>988</v>
       </c>
@@ -8430,7 +8488,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="5" spans="1:5">
+    <row r="5" spans="1:6">
       <c r="A5" t="s">
         <v>989</v>
       </c>
@@ -8445,7 +8503,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="6" spans="1:5">
+    <row r="6" spans="1:6">
       <c r="A6" t="s">
         <v>990</v>
       </c>
@@ -8460,7 +8518,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="7" spans="1:5">
+    <row r="7" spans="1:6">
       <c r="A7" t="s">
         <v>991</v>
       </c>
@@ -8475,7 +8533,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="8" spans="1:5">
+    <row r="8" spans="1:6">
       <c r="A8" t="s">
         <v>992</v>
       </c>
@@ -8490,7 +8548,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="9" spans="1:5">
+    <row r="9" spans="1:6">
       <c r="A9" t="s">
         <v>993</v>
       </c>
@@ -8505,7 +8563,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="10" spans="1:5">
+    <row r="10" spans="1:6">
       <c r="A10" t="s">
         <v>994</v>
       </c>
@@ -8520,7 +8578,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="11" spans="1:5">
+    <row r="11" spans="1:6">
       <c r="A11" t="s">
         <v>995</v>
       </c>
@@ -8535,7 +8593,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="12" spans="1:5">
+    <row r="12" spans="1:6">
       <c r="A12" t="s">
         <v>996</v>
       </c>
@@ -8550,7 +8608,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="13" spans="1:5">
+    <row r="13" spans="1:6">
       <c r="A13" t="s">
         <v>997</v>
       </c>
@@ -8565,7 +8623,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="14" spans="1:5">
+    <row r="14" spans="1:6">
       <c r="A14" t="s">
         <v>998</v>
       </c>
@@ -8580,7 +8638,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="15" spans="1:5">
+    <row r="15" spans="1:6">
       <c r="A15" t="s">
         <v>999</v>
       </c>
@@ -8595,7 +8653,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="16" spans="1:5">
+    <row r="16" spans="1:6">
       <c r="A16" t="s">
         <v>1000</v>
       </c>
@@ -10050,7 +10108,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="113" spans="1:5">
+    <row r="113" spans="1:6">
       <c r="A113" t="s">
         <v>1006</v>
       </c>
@@ -10065,7 +10123,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="114" spans="1:5">
+    <row r="114" spans="1:6">
       <c r="A114" t="s">
         <v>1007</v>
       </c>
@@ -10080,7 +10138,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="115" spans="1:5">
+    <row r="115" spans="1:6">
       <c r="A115" t="s">
         <v>1008</v>
       </c>
@@ -10095,7 +10153,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="116" spans="1:5">
+    <row r="116" spans="1:6">
       <c r="A116" t="s">
         <v>916</v>
       </c>
@@ -10112,8 +10170,11 @@
       <c r="E116" t="s">
         <v>1027</v>
       </c>
-    </row>
-    <row r="117" spans="1:5">
+      <c r="F116" t="s">
+        <v>1240</v>
+      </c>
+    </row>
+    <row r="117" spans="1:6">
       <c r="A117" t="s">
         <v>917</v>
       </c>
@@ -10130,8 +10191,11 @@
       <c r="E117" t="s">
         <v>1027</v>
       </c>
-    </row>
-    <row r="118" spans="1:5">
+      <c r="F117" t="s">
+        <v>1247</v>
+      </c>
+    </row>
+    <row r="118" spans="1:6">
       <c r="A118" t="s">
         <v>918</v>
       </c>
@@ -10148,8 +10212,11 @@
       <c r="E118" t="s">
         <v>1027</v>
       </c>
-    </row>
-    <row r="119" spans="1:5">
+      <c r="F118" t="s">
+        <v>1248</v>
+      </c>
+    </row>
+    <row r="119" spans="1:6">
       <c r="A119" t="s">
         <v>919</v>
       </c>
@@ -10166,8 +10233,11 @@
       <c r="E119" t="s">
         <v>1027</v>
       </c>
-    </row>
-    <row r="120" spans="1:5">
+      <c r="F119" t="s">
+        <v>1249</v>
+      </c>
+    </row>
+    <row r="120" spans="1:6">
       <c r="A120" t="s">
         <v>921</v>
       </c>
@@ -10184,8 +10254,11 @@
       <c r="E120" t="s">
         <v>1027</v>
       </c>
-    </row>
-    <row r="121" spans="1:5">
+      <c r="F120" t="s">
+        <v>1250</v>
+      </c>
+    </row>
+    <row r="121" spans="1:6">
       <c r="A121" t="s">
         <v>922</v>
       </c>
@@ -10202,8 +10275,11 @@
       <c r="E121" t="s">
         <v>1027</v>
       </c>
-    </row>
-    <row r="122" spans="1:5">
+      <c r="F121" t="s">
+        <v>1251</v>
+      </c>
+    </row>
+    <row r="122" spans="1:6">
       <c r="A122" t="s">
         <v>923</v>
       </c>
@@ -10220,8 +10296,11 @@
       <c r="E122" t="s">
         <v>1027</v>
       </c>
-    </row>
-    <row r="123" spans="1:5">
+      <c r="F122" t="s">
+        <v>1252</v>
+      </c>
+    </row>
+    <row r="123" spans="1:6">
       <c r="A123" t="s">
         <v>924</v>
       </c>
@@ -10238,8 +10317,11 @@
       <c r="E123" t="s">
         <v>1027</v>
       </c>
-    </row>
-    <row r="124" spans="1:5">
+      <c r="F123" t="s">
+        <v>1246</v>
+      </c>
+    </row>
+    <row r="124" spans="1:6">
       <c r="A124" t="s">
         <v>926</v>
       </c>
@@ -10256,8 +10338,11 @@
       <c r="E124" t="s">
         <v>1027</v>
       </c>
-    </row>
-    <row r="125" spans="1:5">
+      <c r="F124" t="s">
+        <v>1253</v>
+      </c>
+    </row>
+    <row r="125" spans="1:6">
       <c r="A125" t="s">
         <v>930</v>
       </c>
@@ -10274,8 +10359,11 @@
       <c r="E125" t="s">
         <v>1027</v>
       </c>
-    </row>
-    <row r="126" spans="1:5">
+      <c r="F125" t="s">
+        <v>1243</v>
+      </c>
+    </row>
+    <row r="126" spans="1:6">
       <c r="A126" t="s">
         <v>934</v>
       </c>
@@ -10292,8 +10380,11 @@
       <c r="E126" t="s">
         <v>1027</v>
       </c>
-    </row>
-    <row r="127" spans="1:5">
+      <c r="F126" t="s">
+        <v>1254</v>
+      </c>
+    </row>
+    <row r="127" spans="1:6">
       <c r="A127" t="s">
         <v>935</v>
       </c>
@@ -10310,8 +10401,11 @@
       <c r="E127" t="s">
         <v>1027</v>
       </c>
-    </row>
-    <row r="128" spans="1:5">
+      <c r="F127" t="s">
+        <v>1244</v>
+      </c>
+    </row>
+    <row r="128" spans="1:6">
       <c r="A128" t="s">
         <v>936</v>
       </c>
@@ -10328,8 +10422,11 @@
       <c r="E128" t="s">
         <v>1027</v>
       </c>
-    </row>
-    <row r="129" spans="1:5">
+      <c r="F128" t="s">
+        <v>1245</v>
+      </c>
+    </row>
+    <row r="129" spans="1:6">
       <c r="A129" t="s">
         <v>920</v>
       </c>
@@ -10344,7 +10441,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="130" spans="1:5">
+    <row r="130" spans="1:6">
       <c r="A130" t="s">
         <v>925</v>
       </c>
@@ -10359,7 +10456,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="131" spans="1:5">
+    <row r="131" spans="1:6">
       <c r="A131" t="s">
         <v>927</v>
       </c>
@@ -10374,7 +10471,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="132" spans="1:5">
+    <row r="132" spans="1:6">
       <c r="A132" t="s">
         <v>928</v>
       </c>
@@ -10389,7 +10486,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="133" spans="1:5">
+    <row r="133" spans="1:6">
       <c r="A133" t="s">
         <v>929</v>
       </c>
@@ -10404,7 +10501,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="134" spans="1:5">
+    <row r="134" spans="1:6">
       <c r="A134" t="s">
         <v>931</v>
       </c>
@@ -10419,7 +10516,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="135" spans="1:5">
+    <row r="135" spans="1:6">
       <c r="A135" t="s">
         <v>932</v>
       </c>
@@ -10434,7 +10531,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="136" spans="1:5">
+    <row r="136" spans="1:6">
       <c r="A136" t="s">
         <v>933</v>
       </c>
@@ -10449,7 +10546,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="137" spans="1:5">
+    <row r="137" spans="1:6">
       <c r="A137" t="s">
         <v>937</v>
       </c>
@@ -10464,7 +10561,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="138" spans="1:5">
+    <row r="138" spans="1:6">
       <c r="A138" t="s">
         <v>941</v>
       </c>
@@ -10481,8 +10578,11 @@
       <c r="E138" t="s">
         <v>1027</v>
       </c>
-    </row>
-    <row r="139" spans="1:5">
+      <c r="F138" t="s">
+        <v>1238</v>
+      </c>
+    </row>
+    <row r="139" spans="1:6">
       <c r="A139" t="s">
         <v>938</v>
       </c>
@@ -10497,7 +10597,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="140" spans="1:5">
+    <row r="140" spans="1:6">
       <c r="A140" t="s">
         <v>939</v>
       </c>
@@ -10512,7 +10612,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="141" spans="1:5">
+    <row r="141" spans="1:6">
       <c r="A141" t="s">
         <v>940</v>
       </c>
@@ -10527,7 +10627,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="142" spans="1:5">
+    <row r="142" spans="1:6">
       <c r="A142" t="s">
         <v>942</v>
       </c>
@@ -10542,7 +10642,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="143" spans="1:5">
+    <row r="143" spans="1:6">
       <c r="A143" t="s">
         <v>827</v>
       </c>
@@ -10559,8 +10659,11 @@
       <c r="E143" t="s">
         <v>1027</v>
       </c>
-    </row>
-    <row r="144" spans="1:5">
+      <c r="F143" t="s">
+        <v>1239</v>
+      </c>
+    </row>
+    <row r="144" spans="1:6">
       <c r="A144" t="s">
         <v>824</v>
       </c>
@@ -10575,7 +10678,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="145" spans="1:5">
+    <row r="145" spans="1:6">
       <c r="A145" t="s">
         <v>825</v>
       </c>
@@ -10590,7 +10693,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="146" spans="1:5">
+    <row r="146" spans="1:6">
       <c r="A146" t="s">
         <v>826</v>
       </c>
@@ -10605,7 +10708,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="147" spans="1:5">
+    <row r="147" spans="1:6">
       <c r="A147" t="s">
         <v>828</v>
       </c>
@@ -10620,7 +10723,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="148" spans="1:5">
+    <row r="148" spans="1:6">
       <c r="A148" t="s">
         <v>829</v>
       </c>
@@ -10635,7 +10738,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="149" spans="1:5">
+    <row r="149" spans="1:6">
       <c r="A149" t="s">
         <v>830</v>
       </c>
@@ -10650,7 +10753,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="150" spans="1:5">
+    <row r="150" spans="1:6">
       <c r="A150" t="s">
         <v>831</v>
       </c>
@@ -10665,7 +10768,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="151" spans="1:5">
+    <row r="151" spans="1:6">
       <c r="A151" t="s">
         <v>832</v>
       </c>
@@ -10680,7 +10783,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="152" spans="1:5">
+    <row r="152" spans="1:6">
       <c r="A152" t="s">
         <v>833</v>
       </c>
@@ -10695,7 +10798,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="153" spans="1:5">
+    <row r="153" spans="1:6">
       <c r="A153" t="s">
         <v>834</v>
       </c>
@@ -10712,8 +10815,11 @@
       <c r="E153" t="s">
         <v>1027</v>
       </c>
-    </row>
-    <row r="154" spans="1:5">
+      <c r="F153" t="s">
+        <v>1242</v>
+      </c>
+    </row>
+    <row r="154" spans="1:6">
       <c r="A154" t="s">
         <v>835</v>
       </c>
@@ -10730,8 +10836,11 @@
       <c r="E154" t="s">
         <v>1027</v>
       </c>
-    </row>
-    <row r="155" spans="1:5">
+      <c r="F154" t="s">
+        <v>1242</v>
+      </c>
+    </row>
+    <row r="155" spans="1:6">
       <c r="A155" t="s">
         <v>836</v>
       </c>
@@ -10748,8 +10857,11 @@
       <c r="E155" t="s">
         <v>1027</v>
       </c>
-    </row>
-    <row r="156" spans="1:5">
+      <c r="F155" t="s">
+        <v>1242</v>
+      </c>
+    </row>
+    <row r="156" spans="1:6">
       <c r="A156" t="s">
         <v>837</v>
       </c>
@@ -10766,8 +10878,11 @@
       <c r="E156" t="s">
         <v>1027</v>
       </c>
-    </row>
-    <row r="157" spans="1:5">
+      <c r="F156" t="s">
+        <v>1242</v>
+      </c>
+    </row>
+    <row r="157" spans="1:6">
       <c r="A157" t="s">
         <v>838</v>
       </c>
@@ -10784,8 +10899,11 @@
       <c r="E157" t="s">
         <v>1027</v>
       </c>
-    </row>
-    <row r="158" spans="1:5">
+      <c r="F157" t="s">
+        <v>1242</v>
+      </c>
+    </row>
+    <row r="158" spans="1:6">
       <c r="A158" t="s">
         <v>839</v>
       </c>
@@ -10802,8 +10920,11 @@
       <c r="E158" t="s">
         <v>1027</v>
       </c>
-    </row>
-    <row r="159" spans="1:5">
+      <c r="F158" t="s">
+        <v>1242</v>
+      </c>
+    </row>
+    <row r="159" spans="1:6">
       <c r="A159" t="s">
         <v>840</v>
       </c>
@@ -10820,8 +10941,11 @@
       <c r="E159" t="s">
         <v>1027</v>
       </c>
-    </row>
-    <row r="160" spans="1:5">
+      <c r="F159" t="s">
+        <v>1242</v>
+      </c>
+    </row>
+    <row r="160" spans="1:6">
       <c r="A160" t="s">
         <v>841</v>
       </c>
@@ -10838,8 +10962,11 @@
       <c r="E160" t="s">
         <v>1027</v>
       </c>
-    </row>
-    <row r="161" spans="1:5">
+      <c r="F160" t="s">
+        <v>1242</v>
+      </c>
+    </row>
+    <row r="161" spans="1:6">
       <c r="A161" t="s">
         <v>842</v>
       </c>
@@ -10856,8 +10983,11 @@
       <c r="E161" t="s">
         <v>1027</v>
       </c>
-    </row>
-    <row r="162" spans="1:5">
+      <c r="F161" t="s">
+        <v>1242</v>
+      </c>
+    </row>
+    <row r="162" spans="1:6">
       <c r="A162" t="s">
         <v>843</v>
       </c>
@@ -10874,8 +11004,11 @@
       <c r="E162" t="s">
         <v>1027</v>
       </c>
-    </row>
-    <row r="163" spans="1:5">
+      <c r="F162" t="s">
+        <v>1242</v>
+      </c>
+    </row>
+    <row r="163" spans="1:6">
       <c r="A163" t="s">
         <v>844</v>
       </c>
@@ -10892,8 +11025,11 @@
       <c r="E163" t="s">
         <v>1027</v>
       </c>
-    </row>
-    <row r="164" spans="1:5">
+      <c r="F163" t="s">
+        <v>1242</v>
+      </c>
+    </row>
+    <row r="164" spans="1:6">
       <c r="A164" t="s">
         <v>845</v>
       </c>
@@ -10910,8 +11046,11 @@
       <c r="E164" t="s">
         <v>1027</v>
       </c>
-    </row>
-    <row r="165" spans="1:5">
+      <c r="F164" t="s">
+        <v>1242</v>
+      </c>
+    </row>
+    <row r="165" spans="1:6">
       <c r="A165" t="s">
         <v>846</v>
       </c>
@@ -10928,8 +11067,11 @@
       <c r="E165" t="s">
         <v>1027</v>
       </c>
-    </row>
-    <row r="166" spans="1:5">
+      <c r="F165" t="s">
+        <v>1242</v>
+      </c>
+    </row>
+    <row r="166" spans="1:6">
       <c r="A166" t="s">
         <v>847</v>
       </c>
@@ -10946,8 +11088,11 @@
       <c r="E166" t="s">
         <v>1027</v>
       </c>
-    </row>
-    <row r="167" spans="1:5">
+      <c r="F166" t="s">
+        <v>1242</v>
+      </c>
+    </row>
+    <row r="167" spans="1:6">
       <c r="A167" t="s">
         <v>848</v>
       </c>
@@ -10964,8 +11109,11 @@
       <c r="E167" t="s">
         <v>1027</v>
       </c>
-    </row>
-    <row r="168" spans="1:5">
+      <c r="F167" t="s">
+        <v>1242</v>
+      </c>
+    </row>
+    <row r="168" spans="1:6">
       <c r="A168" t="s">
         <v>849</v>
       </c>
@@ -10982,8 +11130,11 @@
       <c r="E168" t="s">
         <v>1027</v>
       </c>
-    </row>
-    <row r="169" spans="1:5">
+      <c r="F168" t="s">
+        <v>1242</v>
+      </c>
+    </row>
+    <row r="169" spans="1:6">
       <c r="A169" t="s">
         <v>850</v>
       </c>
@@ -11000,8 +11151,11 @@
       <c r="E169" t="s">
         <v>1027</v>
       </c>
-    </row>
-    <row r="170" spans="1:5">
+      <c r="F169" t="s">
+        <v>1242</v>
+      </c>
+    </row>
+    <row r="170" spans="1:6">
       <c r="A170" t="s">
         <v>851</v>
       </c>
@@ -11018,8 +11172,11 @@
       <c r="E170" t="s">
         <v>1027</v>
       </c>
-    </row>
-    <row r="171" spans="1:5">
+      <c r="F170" t="s">
+        <v>1242</v>
+      </c>
+    </row>
+    <row r="171" spans="1:6">
       <c r="A171" t="s">
         <v>852</v>
       </c>
@@ -11036,8 +11193,11 @@
       <c r="E171" t="s">
         <v>1027</v>
       </c>
-    </row>
-    <row r="172" spans="1:5">
+      <c r="F171" t="s">
+        <v>1242</v>
+      </c>
+    </row>
+    <row r="172" spans="1:6">
       <c r="A172" t="s">
         <v>853</v>
       </c>
@@ -11054,8 +11214,11 @@
       <c r="E172" t="s">
         <v>1027</v>
       </c>
-    </row>
-    <row r="173" spans="1:5">
+      <c r="F172" t="s">
+        <v>1242</v>
+      </c>
+    </row>
+    <row r="173" spans="1:6">
       <c r="A173" t="s">
         <v>854</v>
       </c>
@@ -11072,8 +11235,11 @@
       <c r="E173" t="s">
         <v>1027</v>
       </c>
-    </row>
-    <row r="174" spans="1:5">
+      <c r="F173" t="s">
+        <v>1242</v>
+      </c>
+    </row>
+    <row r="174" spans="1:6">
       <c r="A174" t="s">
         <v>855</v>
       </c>
@@ -11090,8 +11256,11 @@
       <c r="E174" t="s">
         <v>1027</v>
       </c>
-    </row>
-    <row r="175" spans="1:5">
+      <c r="F174" t="s">
+        <v>1242</v>
+      </c>
+    </row>
+    <row r="175" spans="1:6">
       <c r="A175" t="s">
         <v>856</v>
       </c>
@@ -11108,8 +11277,11 @@
       <c r="E175" t="s">
         <v>1027</v>
       </c>
-    </row>
-    <row r="176" spans="1:5">
+      <c r="F175" t="s">
+        <v>1242</v>
+      </c>
+    </row>
+    <row r="176" spans="1:6">
       <c r="A176" t="s">
         <v>857</v>
       </c>
@@ -11126,8 +11298,11 @@
       <c r="E176" t="s">
         <v>1027</v>
       </c>
-    </row>
-    <row r="177" spans="1:5">
+      <c r="F176" t="s">
+        <v>1242</v>
+      </c>
+    </row>
+    <row r="177" spans="1:6">
       <c r="A177" t="s">
         <v>858</v>
       </c>
@@ -11144,8 +11319,11 @@
       <c r="E177" t="s">
         <v>1027</v>
       </c>
-    </row>
-    <row r="178" spans="1:5">
+      <c r="F177" t="s">
+        <v>1242</v>
+      </c>
+    </row>
+    <row r="178" spans="1:6">
       <c r="A178" t="s">
         <v>859</v>
       </c>
@@ -11162,8 +11340,11 @@
       <c r="E178" t="s">
         <v>1027</v>
       </c>
-    </row>
-    <row r="179" spans="1:5">
+      <c r="F178" t="s">
+        <v>1242</v>
+      </c>
+    </row>
+    <row r="179" spans="1:6">
       <c r="A179" t="s">
         <v>860</v>
       </c>
@@ -11180,8 +11361,11 @@
       <c r="E179" t="s">
         <v>1027</v>
       </c>
-    </row>
-    <row r="180" spans="1:5">
+      <c r="F179" t="s">
+        <v>1242</v>
+      </c>
+    </row>
+    <row r="180" spans="1:6">
       <c r="A180" t="s">
         <v>861</v>
       </c>
@@ -11198,8 +11382,11 @@
       <c r="E180" t="s">
         <v>1027</v>
       </c>
-    </row>
-    <row r="181" spans="1:5">
+      <c r="F180" t="s">
+        <v>1242</v>
+      </c>
+    </row>
+    <row r="181" spans="1:6">
       <c r="A181" t="s">
         <v>862</v>
       </c>
@@ -11216,8 +11403,11 @@
       <c r="E181" t="s">
         <v>1027</v>
       </c>
-    </row>
-    <row r="182" spans="1:5">
+      <c r="F181" t="s">
+        <v>1242</v>
+      </c>
+    </row>
+    <row r="182" spans="1:6">
       <c r="A182" t="s">
         <v>863</v>
       </c>
@@ -11234,8 +11424,11 @@
       <c r="E182" t="s">
         <v>1027</v>
       </c>
-    </row>
-    <row r="183" spans="1:5">
+      <c r="F182" t="s">
+        <v>1242</v>
+      </c>
+    </row>
+    <row r="183" spans="1:6">
       <c r="A183" t="s">
         <v>864</v>
       </c>
@@ -11252,8 +11445,11 @@
       <c r="E183" t="s">
         <v>1027</v>
       </c>
-    </row>
-    <row r="184" spans="1:5">
+      <c r="F183" t="s">
+        <v>1242</v>
+      </c>
+    </row>
+    <row r="184" spans="1:6">
       <c r="A184" t="s">
         <v>865</v>
       </c>
@@ -11270,8 +11466,11 @@
       <c r="E184" t="s">
         <v>1027</v>
       </c>
-    </row>
-    <row r="185" spans="1:5">
+      <c r="F184" t="s">
+        <v>1242</v>
+      </c>
+    </row>
+    <row r="185" spans="1:6">
       <c r="A185" t="s">
         <v>866</v>
       </c>
@@ -11288,8 +11487,11 @@
       <c r="E185" t="s">
         <v>1027</v>
       </c>
-    </row>
-    <row r="186" spans="1:5">
+      <c r="F185" t="s">
+        <v>1242</v>
+      </c>
+    </row>
+    <row r="186" spans="1:6">
       <c r="A186" t="s">
         <v>867</v>
       </c>
@@ -11306,8 +11508,11 @@
       <c r="E186" t="s">
         <v>1027</v>
       </c>
-    </row>
-    <row r="187" spans="1:5">
+      <c r="F186" t="s">
+        <v>1242</v>
+      </c>
+    </row>
+    <row r="187" spans="1:6">
       <c r="A187" t="s">
         <v>868</v>
       </c>
@@ -11324,8 +11529,11 @@
       <c r="E187" t="s">
         <v>1027</v>
       </c>
-    </row>
-    <row r="188" spans="1:5">
+      <c r="F187" t="s">
+        <v>1242</v>
+      </c>
+    </row>
+    <row r="188" spans="1:6">
       <c r="A188" t="s">
         <v>869</v>
       </c>
@@ -11342,8 +11550,11 @@
       <c r="E188" t="s">
         <v>1027</v>
       </c>
-    </row>
-    <row r="189" spans="1:5">
+      <c r="F188" t="s">
+        <v>1242</v>
+      </c>
+    </row>
+    <row r="189" spans="1:6">
       <c r="A189" t="s">
         <v>870</v>
       </c>
@@ -11360,8 +11571,11 @@
       <c r="E189" t="s">
         <v>1027</v>
       </c>
-    </row>
-    <row r="190" spans="1:5">
+      <c r="F189" t="s">
+        <v>1242</v>
+      </c>
+    </row>
+    <row r="190" spans="1:6">
       <c r="A190" t="s">
         <v>871</v>
       </c>
@@ -11378,8 +11592,11 @@
       <c r="E190" t="s">
         <v>1027</v>
       </c>
-    </row>
-    <row r="191" spans="1:5">
+      <c r="F190" t="s">
+        <v>1242</v>
+      </c>
+    </row>
+    <row r="191" spans="1:6">
       <c r="A191" t="s">
         <v>872</v>
       </c>
@@ -11396,8 +11613,11 @@
       <c r="E191" t="s">
         <v>1027</v>
       </c>
-    </row>
-    <row r="192" spans="1:5">
+      <c r="F191" t="s">
+        <v>1241</v>
+      </c>
+    </row>
+    <row r="192" spans="1:6">
       <c r="A192" t="s">
         <v>873</v>
       </c>
@@ -11414,8 +11634,11 @@
       <c r="E192" t="s">
         <v>1027</v>
       </c>
-    </row>
-    <row r="193" spans="1:5">
+      <c r="F192" t="s">
+        <v>1241</v>
+      </c>
+    </row>
+    <row r="193" spans="1:6">
       <c r="A193" t="s">
         <v>874</v>
       </c>
@@ -11432,8 +11655,11 @@
       <c r="E193" t="s">
         <v>1027</v>
       </c>
-    </row>
-    <row r="194" spans="1:5">
+      <c r="F193" t="s">
+        <v>1241</v>
+      </c>
+    </row>
+    <row r="194" spans="1:6">
       <c r="A194" t="s">
         <v>875</v>
       </c>
@@ -11450,8 +11676,11 @@
       <c r="E194" t="s">
         <v>1027</v>
       </c>
-    </row>
-    <row r="195" spans="1:5">
+      <c r="F194" t="s">
+        <v>1241</v>
+      </c>
+    </row>
+    <row r="195" spans="1:6">
       <c r="A195" t="s">
         <v>876</v>
       </c>
@@ -11468,8 +11697,11 @@
       <c r="E195" t="s">
         <v>1027</v>
       </c>
-    </row>
-    <row r="196" spans="1:5">
+      <c r="F195" t="s">
+        <v>1241</v>
+      </c>
+    </row>
+    <row r="196" spans="1:6">
       <c r="A196" t="s">
         <v>877</v>
       </c>
@@ -11486,8 +11718,11 @@
       <c r="E196" t="s">
         <v>1027</v>
       </c>
-    </row>
-    <row r="197" spans="1:5">
+      <c r="F196" t="s">
+        <v>1241</v>
+      </c>
+    </row>
+    <row r="197" spans="1:6">
       <c r="A197" t="s">
         <v>878</v>
       </c>
@@ -11504,8 +11739,11 @@
       <c r="E197" t="s">
         <v>1027</v>
       </c>
-    </row>
-    <row r="198" spans="1:5">
+      <c r="F197" t="s">
+        <v>1241</v>
+      </c>
+    </row>
+    <row r="198" spans="1:6">
       <c r="A198" t="s">
         <v>879</v>
       </c>
@@ -11522,8 +11760,11 @@
       <c r="E198" t="s">
         <v>1027</v>
       </c>
-    </row>
-    <row r="199" spans="1:5">
+      <c r="F198" t="s">
+        <v>1241</v>
+      </c>
+    </row>
+    <row r="199" spans="1:6">
       <c r="A199" t="s">
         <v>880</v>
       </c>
@@ -11540,48 +11781,51 @@
       <c r="E199" t="s">
         <v>1027</v>
       </c>
-    </row>
-    <row r="200" spans="1:5">
+      <c r="F199" t="s">
+        <v>1241</v>
+      </c>
+    </row>
+    <row r="200" spans="1:6">
       <c r="A200" s="1"/>
       <c r="B200" s="1"/>
       <c r="C200" s="1"/>
     </row>
-    <row r="201" spans="1:5">
+    <row r="201" spans="1:6">
       <c r="A201" s="1"/>
       <c r="B201" s="1"/>
       <c r="C201" s="1"/>
     </row>
-    <row r="202" spans="1:5">
+    <row r="202" spans="1:6">
       <c r="A202" s="1"/>
       <c r="B202" s="1"/>
       <c r="C202" s="1"/>
     </row>
-    <row r="203" spans="1:5">
+    <row r="203" spans="1:6">
       <c r="A203" s="1"/>
       <c r="B203" s="1"/>
       <c r="C203" s="1"/>
     </row>
-    <row r="204" spans="1:5">
+    <row r="204" spans="1:6">
       <c r="A204" s="1"/>
       <c r="B204" s="1"/>
       <c r="C204" s="1"/>
     </row>
-    <row r="205" spans="1:5">
+    <row r="205" spans="1:6">
       <c r="A205" s="1"/>
       <c r="B205" s="1"/>
       <c r="C205" s="1"/>
     </row>
-    <row r="206" spans="1:5">
+    <row r="206" spans="1:6">
       <c r="A206" s="1"/>
       <c r="B206" s="1"/>
       <c r="C206" s="1"/>
     </row>
-    <row r="207" spans="1:5">
+    <row r="207" spans="1:6">
       <c r="A207" s="1"/>
       <c r="B207" s="1"/>
       <c r="C207" s="1"/>
     </row>
-    <row r="208" spans="1:5">
+    <row r="208" spans="1:6">
       <c r="A208" s="1"/>
       <c r="B208" s="1"/>
       <c r="C208" s="1"/>

</xml_diff>